<commit_message>
fixed xlsx data not being identified as strings
</commit_message>
<xml_diff>
--- a/video_data.xlsx
+++ b/video_data.xlsx
@@ -65,7 +65,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -424,12 +424,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="9.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">

</xml_diff>

<commit_message>
added handling of extraneous empty cells
</commit_message>
<xml_diff>
--- a/video_data.xlsx
+++ b/video_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>FILENAME</t>
   </si>
@@ -40,13 +40,7 @@
     <t>00:00:00</t>
   </si>
   <si>
-    <t>Line_1</t>
-  </si>
-  <si>
-    <t>Line_2</t>
-  </si>
-  <si>
-    <t>Line_3</t>
+    <t>Example</t>
   </si>
 </sst>
 </file>
@@ -466,10 +460,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved audio fade between clips
</commit_message>
<xml_diff>
--- a/video_data.xlsx
+++ b/video_data.xlsx
@@ -47,17 +47,18 @@
     <t xml:space="preserve">00:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">Example</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -133,28 +134,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,14 +193,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.58"/>
@@ -217,399 +230,399 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -624,8 +637,8 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -640,8 +653,8 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -656,8 +669,8 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -672,8 +685,8 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -688,8 +701,8 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -704,8 +717,8 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -720,8 +733,8 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -736,8 +749,8 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -752,8 +765,8 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -768,8 +781,8 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -784,8 +797,8 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -800,8 +813,8 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -816,8 +829,8 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -832,8 +845,8 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -848,8 +861,8 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>

</xml_diff>